<commit_message>
bang phân công mới
</commit_message>
<xml_diff>
--- a/Phân công công việc/Phân công công việc 1805.xlsx
+++ b/Phân công công việc/Phân công công việc 1805.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Quốc + Tâm: Thiết Kế CSDL access</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>Quốc :Màn Hình Chính &amp; Màn Hình Phục Vụ</t>
-  </si>
-  <si>
-    <t>INF</t>
   </si>
   <si>
     <t>Thiết kế Xử Lý Màn hình Chính &amp; màn phục vụ(Đổi Tách Ghép Bàn, Tính Tiền), Viết các lớp DTO, Các cài đặt phụ cho phần mềm</t>
@@ -250,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -338,84 +335,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -425,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -455,13 +374,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -475,37 +392,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1760,10 +1648,10 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="18"/>
+      <c r="B21" s="15"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -1826,7 +1714,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1848,28 +1736,28 @@
       <c r="A3" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19" t="s">
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="17"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="6" t="s">
         <v>23</v>
       </c>
@@ -1884,7 +1772,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20">
+      <c r="A8" s="18">
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1903,7 +1791,7 @@
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="7" t="str">
         <f>+B8</f>
         <v>Thiết kế cơ sở dữ liệu</v>
@@ -1921,7 +1809,7 @@
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
@@ -1938,7 +1826,7 @@
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="7" t="str">
         <f>+B10</f>
         <v xml:space="preserve">Thiết kế màn hình Axure </v>
@@ -1967,7 +1855,7 @@
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20">
+      <c r="A13" s="18">
         <v>2</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1986,7 +1874,7 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
@@ -2003,7 +1891,7 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="7" t="s">
         <v>29</v>
       </c>
@@ -2020,7 +1908,7 @@
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="13" t="s">
         <v>30</v>
       </c>
@@ -2037,11 +1925,11 @@
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20">
+      <c r="A17" s="18">
         <v>3</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>35</v>
@@ -2050,19 +1938,19 @@
         <v>41419</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="17" t="s">
-        <v>39</v>
+      <c r="F17" s="9">
+        <v>41311</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="34" t="s">
-        <v>45</v>
+      <c r="H17" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
+    <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
       <c r="B18" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>36</v>
@@ -2071,75 +1959,75 @@
         <v>41419</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="17" t="s">
-        <v>39</v>
+      <c r="F18" s="9">
+        <v>41311</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="34"/>
-    </row>
-    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="23" t="s">
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="19"/>
+      <c r="B19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="9">
+        <v>41419</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9">
+        <v>41311</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="19"/>
+      <c r="B20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="27">
+      <c r="C20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="9">
         <v>41419</v>
       </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="34"/>
-    </row>
-    <row r="20" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="34"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="9">
+        <v>41311</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="15">
+        <v>33</v>
+      </c>
+      <c r="D21" s="9">
         <v>41419</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="F21" s="17" t="s">
-        <v>39</v>
+      <c r="F21" s="9">
+        <v>41311</v>
       </c>
       <c r="G21" s="7"/>
-      <c r="H21" s="34"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
-      <c r="B22" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="16">
-        <v>41419</v>
-      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="F22" s="14"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="34"/>
+      <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
@@ -2159,7 +2047,7 @@
       <c r="F24" s="14"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -2170,12 +2058,6 @@
     </row>
     <row r="26" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2189,17 +2071,11 @@
     <filterColumn colId="5" showButton="0"/>
   </autoFilter>
   <dataConsolidate/>
-  <mergeCells count="15">
+  <mergeCells count="9">
     <mergeCell ref="H17:H22"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="G19:G20"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A6:A7"/>
@@ -2207,7 +2083,7 @@
     <mergeCell ref="C6:C7"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J17 C8:C19 C21:C26">
+    <dataValidation type="list" imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J17 C8:C19 C20:C25">
       <formula1>Staff</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>